<commit_message>
Funcional resistence/support validation implemented
</commit_message>
<xml_diff>
--- a/files/winm20_streaming.xlsx
+++ b/files/winm20_streaming.xlsx
@@ -5,9 +5,44 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Planilha1" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+  <si>
+    <t>Fundos</t>
+  </si>
+  <si>
+    <t>Topos</t>
+  </si>
+  <si>
+    <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Nome da acao</t>
+  </si>
+  <si>
+    <t>Valor atual</t>
+  </si>
+  <si>
+    <t>2020-05-14T23:20:56.592Z</t>
+  </si>
+  <si>
+    <t>WINM20</t>
+  </si>
+  <si>
+    <t>2020-05-15T23:20:56.592Z</t>
+  </si>
+  <si>
+    <t>2020-05-16T23:20:56.592Z</t>
+  </si>
+  <si>
+    <t>2020-05-17T23:20:56.592Z</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15,16 +50,11 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
@@ -32,9 +62,20 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="14"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -46,12 +87,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -61,16 +102,60 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -80,17 +165,38 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -111,6 +217,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff70ad47"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -118,9 +225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office Theme">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
@@ -134,22 +241,22 @@
         <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -158,7 +265,7 @@
         <a:srgbClr val="FF00FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office Theme">
       <a:majorFont>
         <a:latin typeface="Helvetica Neue"/>
         <a:ea typeface="Helvetica Neue"/>
@@ -170,7 +277,7 @@
         <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office Theme">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -249,13 +356,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -316,17 +417,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -354,10 +455,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -605,20 +706,14 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -903,7 +998,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -931,10 +1026,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="Calibri"/>
+            <a:ea typeface="Calibri"/>
+            <a:cs typeface="Calibri"/>
+            <a:sym typeface="Calibri"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1189,89 +1284,128 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="12.8" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="11.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="22" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="1" customWidth="1"/>
     <col min="6" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="2">
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="5">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5">
+        <v>500</v>
+      </c>
+      <c r="C2" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5">
+        <v>130.84</v>
+      </c>
     </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="7">
+        <v>100</v>
+      </c>
+      <c r="B3" s="7">
+        <v>600</v>
+      </c>
+      <c r="C3" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="7">
+        <v>300</v>
+      </c>
+      <c r="B4" s="7">
+        <v>700</v>
+      </c>
+      <c r="C4" t="s" s="8">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="7">
+        <v>400</v>
+      </c>
+      <c r="B5" s="7">
+        <v>800</v>
+      </c>
+      <c r="C5" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
     </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;K000000Sheet1</oddHeader>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>